<commit_message>
add planing and report
</commit_message>
<xml_diff>
--- a/docs/20140315_ListScreen.xlsx
+++ b/docs/20140315_ListScreen.xlsx
@@ -469,9 +469,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -481,6 +478,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -791,7 +791,7 @@
   <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,12 +815,12 @@
       <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
@@ -831,19 +831,19 @@
       </c>
       <c r="C2" s="12"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="22"/>
+      <c r="C3" s="21"/>
       <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
@@ -869,13 +869,13 @@
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="22"/>
+      <c r="C5" s="21"/>
       <c r="F5" s="1" t="s">
         <v>6</v>
       </c>
@@ -887,17 +887,17 @@
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="22"/>
+      <c r="C6" s="21"/>
       <c r="F6" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G6" s="19"/>
+      <c r="G6" s="18"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -1142,13 +1142,13 @@
       <c r="C27" s="8"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="22"/>
+      <c r="C28" s="21"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>

</xml_diff>